<commit_message>
fix: update cut-off score
</commit_message>
<xml_diff>
--- a/Final Scorecard.xlsx
+++ b/Final Scorecard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ystan\Documents\GitHub\FA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shuoan\Desktop\Financial Analytics\Project\FA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B46AD63-F88C-43A1-B0BB-F31FD29A2650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8B63CE-9A3E-43AC-B801-FE8A298FFA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Scorecard" sheetId="1" r:id="rId1"/>
@@ -1143,20 +1143,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="23.08984375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="1" width="37.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -1164,15 +1164,15 @@
         <v>514</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="5">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>-29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="7" t="s">
         <v>42</v>
@@ -1212,7 +1212,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="7" t="s">
         <v>43</v>
@@ -1224,7 +1224,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="7" t="s">
         <v>44</v>
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="7" t="s">
         <v>2</v>
@@ -1248,7 +1248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>3</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="7" t="s">
         <v>5</v>
@@ -1274,7 +1274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="7" t="s">
         <v>45</v>
@@ -1300,7 +1300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="7" t="s">
         <v>46</v>
@@ -1312,7 +1312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="7" t="s">
         <v>47</v>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="7" t="s">
         <v>8</v>
@@ -1336,7 +1336,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="7" t="s">
         <v>48</v>
@@ -1362,7 +1362,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="7" t="s">
         <v>11</v>
@@ -1374,7 +1374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="7" t="s">
         <v>49</v>
@@ -1400,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="7" t="s">
         <v>14</v>
@@ -1412,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="7" t="s">
         <v>17</v>
@@ -1438,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>18</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
         <v>50</v>
@@ -1464,7 +1464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="7" t="s">
         <v>19</v>
@@ -1476,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>20</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="7" t="s">
         <v>22</v>
@@ -1502,7 +1502,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>23</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="7" t="s">
         <v>51</v>
@@ -1528,7 +1528,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="7" t="s">
         <v>52</v>
@@ -1540,7 +1540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
         <v>53</v>
@@ -1552,7 +1552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="7" t="s">
         <v>54</v>
@@ -1564,7 +1564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
       <c r="B35" s="7" t="s">
         <v>25</v>
@@ -1576,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>26</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="7" t="s">
         <v>22</v>
@@ -1602,7 +1602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>27</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="7" t="s">
         <v>55</v>
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
       <c r="B40" s="7" t="s">
         <v>22</v>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>29</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="7" t="s">
         <v>56</v>
@@ -1666,7 +1666,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
         <v>57</v>
@@ -1678,7 +1678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="7" t="s">
         <v>31</v>
@@ -1690,7 +1690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>32</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="7" t="s">
         <v>5</v>
@@ -1716,7 +1716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>33</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="7" t="s">
         <v>58</v>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="10"/>
       <c r="B49" s="7" t="s">
         <v>46</v>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="7" t="s">
         <v>47</v>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="9"/>
       <c r="B51" s="7" t="s">
         <v>8</v>
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>35</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
       <c r="B53" s="7" t="s">
         <v>5</v>
@@ -1806,6 +1806,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
@@ -1815,12 +1821,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>